<commit_message>
updated giglist to fix broken image links
</commit_message>
<xml_diff>
--- a/public/GigList.xlsx
+++ b/public/GigList.xlsx
@@ -544,7 +544,7 @@
     <t>https://www.3dhubs.com/list-your-service</t>
   </si>
   <si>
-    <t>https://pbs.twimg.com/profile_images/459655442361114624/g2R4h-8j_400x400.png</t>
+    <t>https://scontent.fsan1-2.fna.fbcdn.net/v/t1.0-9/26908027_1621424537923368_5918209827921647228_n.png?oh=f4b7f5afa503075fe335029a2dfdf133&amp;oe=5B1CDE87</t>
   </si>
   <si>
     <t>Closet Collective</t>
@@ -574,7 +574,7 @@
     <t>http://www.eatwith.com/brand/be-a-host/</t>
   </si>
   <si>
-    <t>https://pbs.twimg.com/profile_images/580834291556323328/3nMAphL9_400x400.png</t>
+    <t>https://lh3.googleusercontent.com/odKcksJKOkVgeqXoGmohHVISXKCLNwr0SdqCB6Wf-ReeiV2N1geBYNAv1pxsUAzADg=w300-rw</t>
   </si>
   <si>
     <t>Josephine</t>
@@ -733,7 +733,7 @@
     <t>https://www.openairplane.com/accounts/register/</t>
   </si>
   <si>
-    <t>https://pbs.twimg.com/profile_images/934115678709342208/PHaVRbZE_400x400.jpg</t>
+    <t>https://scontent.fsan1-2.fna.fbcdn.net/v/t1.0-9/562912_354060034646583_1720132499_n.jpg?oh=fc2d25bfe4d0182ccca518449f89a3db&amp;oe=5B235EE7</t>
   </si>
   <si>
     <t>Uber</t>

</xml_diff>